<commit_message>
feat: Phase 1 - DB 스키마 확장 (3대 주요 기능)
## 1. 의사 조합 템플릿 개선
- Doctor 모델에 shortName 추가 (조합명용 줄임표시)
- DoctorCategory 모델에 shortName 추가
- 엑셀 템플릿 파일 추가: public/templates/doctor-combination-template.xlsx

## 2. 구분별 슬롯 관리 시스템
- CategoryRatioSettings 모델 추가 (구분별 필요인원 비율)
- Staff 모델에 배치 유연성 필드 추가:
  - flexibleForCategories: 다른 구분으로도 배치 가능
  - flexibilityPriority: 유연 배치 우선순위
  - position: 직급 필드
- LeaveApplication에 ON_HOLD, REJECTED 상태 추가
- holdReason 필드 추가 (보류 사유)

## 3. 공휴일 전후 형평성 관리
- 이전 커밋에서 이미 완료:
  - FairnessScore에 holidayAdjacentCount 추가
  - FairnessSettings에 enableHolidayAdjacentFairness 추가

## 마이그레이션
- 20251024234000_add_major_features

다음 단계:
- Phase 2: 서비스 레이어 구현
- Phase 3: 초기 설정 UI 수정

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/의사조합_템플릿.xlsx
+++ b/docs/의사조합_템플릿.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
   <si>
     <t>조합명</t>
   </si>
@@ -41,9 +41,6 @@
     <t>의사명</t>
   </si>
   <si>
-    <t>박창범(상담)</t>
-  </si>
-  <si>
     <t>황우상</t>
   </si>
   <si>
@@ -56,18 +53,6 @@
     <t>윤아향</t>
   </si>
   <si>
-    <t>박창범(진료)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>박(상담)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>박(진료)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>황</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -84,11 +69,53 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구윤진</t>
+    <t>화요일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>야간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목요일</t>
+  </si>
+  <si>
+    <t>목요일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금요일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토요일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박창범</t>
+  </si>
+  <si>
+    <t>박창범</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -465,22 +492,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="6" width="15.77734375" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="7" width="15.77734375" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,128 +515,427 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="str">
-        <f>VLOOKUP(D2,의사목록!$A:$B,2,FALSE) &amp; VLOOKUP(E2,의사목록!$A:$B,2,FALSE) &amp; VLOOKUP(F2,의사목록!$A:$B,2,FALSE)</f>
-        <v>박(상담)구진</v>
+        <f>IF(G2="",VLOOKUP(E2,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F2,의사목록!$A:$B,2,FALSE),VLOOKUP(E2,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F2,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G2,의사목록!$A:$B,2,FALSE))</f>
+        <v>박구윤</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2">
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25">
+    <row r="3" spans="1:9">
+      <c r="A3" t="str">
+        <f>IF(G3="",VLOOKUP(E3,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F3,의사목록!$A:$B,2,FALSE),VLOOKUP(E3,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F3,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G3,의사목록!$A:$B,2,FALSE))</f>
+        <v>구윤</v>
+      </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="str">
+        <f>IF(G4="",VLOOKUP(E4,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F4,의사목록!$A:$B,2,FALSE),VLOOKUP(E4,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F4,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G4,의사목록!$A:$B,2,FALSE))</f>
+        <v>박구윤</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="str">
+        <f>IF(G5="",VLOOKUP(E5,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F5,의사목록!$A:$B,2,FALSE),VLOOKUP(E5,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F5,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G5,의사목록!$A:$B,2,FALSE))</f>
+        <v>박구황</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="str">
+        <f>IF(G6="",VLOOKUP(E6,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F6,의사목록!$A:$B,2,FALSE),VLOOKUP(E6,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F6,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G6,의사목록!$A:$B,2,FALSE))</f>
+        <v>박황윤</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="str">
+        <f>IF(G7="",VLOOKUP(E7,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F7,의사목록!$A:$B,2,FALSE),VLOOKUP(E7,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F7,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G7,의사목록!$A:$B,2,FALSE))</f>
+        <v>박효윤</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="str">
+        <f>IF(G8="",VLOOKUP(E8,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F8,의사목록!$A:$B,2,FALSE),VLOOKUP(E8,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F8,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G8,의사목록!$A:$B,2,FALSE))</f>
+        <v>구윤</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="str">
+        <f>IF(G9="",VLOOKUP(E9,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F9,의사목록!$A:$B,2,FALSE),VLOOKUP(E9,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F9,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G9,의사목록!$A:$B,2,FALSE))</f>
+        <v>효윤</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="str">
+        <f>IF(G10="",VLOOKUP(E10,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F10,의사목록!$A:$B,2,FALSE),VLOOKUP(E10,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F10,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G10,의사목록!$A:$B,2,FALSE))</f>
+        <v>박구효</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="str">
+        <f>IF(G11="",VLOOKUP(E11,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F11,의사목록!$A:$B,2,FALSE),VLOOKUP(E11,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F11,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G11,의사목록!$A:$B,2,FALSE))</f>
+        <v>구효</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="str">
+        <f>IF(G12="",VLOOKUP(E12,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F12,의사목록!$A:$B,2,FALSE),VLOOKUP(E12,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F12,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G12,의사목록!$A:$B,2,FALSE))</f>
+        <v>박황</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="str">
+        <f>IF(G13="",VLOOKUP(E13,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F13,의사목록!$A:$B,2,FALSE),VLOOKUP(E13,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F13,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G13,의사목록!$A:$B,2,FALSE))</f>
+        <v>박구효</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="str">
+        <f>IF(G14="",VLOOKUP(E14,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F14,의사목록!$A:$B,2,FALSE),VLOOKUP(E14,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F14,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G14,의사목록!$A:$B,2,FALSE))</f>
+        <v>박구황</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="str">
+        <f>IF(G15="",VLOOKUP(E15,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F15,의사목록!$A:$B,2,FALSE),VLOOKUP(E15,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F15,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G15,의사목록!$A:$B,2,FALSE))</f>
+        <v>박구</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="str">
+        <f>IF(G16="",VLOOKUP(E16,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F16,의사목록!$A:$B,2,FALSE),VLOOKUP(E16,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F16,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G16,의사목록!$A:$B,2,FALSE))</f>
+        <v>구황</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="str">
+        <f>IF(G17="",VLOOKUP(E17,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F17,의사목록!$A:$B,2,FALSE),VLOOKUP(E17,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(F17,의사목록!$A:$B,2,FALSE)&amp;VLOOKUP(G17,의사목록!$A:$B,2,FALSE))</f>
+        <v>구효</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:G1048576">
       <formula1>의사목록!$A:$A</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 B3:C3 B2:C2" numberStoredAsText="1"/>
+    <ignoredError sqref="D1 B2:B3 A1:B1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +943,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A4:A7 A1:A2" numberStoredAsText="1"/>
+    <ignoredError sqref="A3:A6 A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>